<commit_message>
Data Analysis and slide
</commit_message>
<xml_diff>
--- a/DataAnalysis/FrequencyDrift2021-07-21trial3.xlsx
+++ b/DataAnalysis/FrequencyDrift2021-07-21trial3.xlsx
@@ -8,39 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottezehnder/Documents/Academic/Summer 2021 Phys REU/laserStabilization/DataAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1020D63D-6484-934A-8837-28D7D79724AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7121A182-4C16-B241-8CCA-6DF10C39A238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15740"/>
+    <workbookView xWindow="6360" yWindow="460" windowWidth="28040" windowHeight="16740"/>
   </bookViews>
   <sheets>
-    <sheet name="FrequencyDrift2021-07-21trail3" sheetId="1" r:id="rId1"/>
+    <sheet name="FrequencyDrift2021-07-22trial7" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sweep Expansion</t>
-  </si>
-  <si>
-    <t>Set Current</t>
-  </si>
-  <si>
-    <t>Power (mW)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11.67\</t>
-  </si>
-  <si>
-    <t>t (s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Frequency Drift (GHz)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Active Current (mA) </t>
   </si>
   <si>
     <t>P</t>
@@ -53,6 +35,18 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>t (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Frequency Drift (GHz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Active Current (mA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Piezo Volta </t>
   </si>
 </sst>
 </file>
@@ -642,25 +636,26 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.8145191805257755E-2"/>
-          <c:y val="6.0073740782402192E-2"/>
-          <c:w val="0.91116068157384222"/>
-          <c:h val="0.89095238095238094"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'FrequencyDrift2021-07-22trial7'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Frequency Drift (GHz)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -695,6 +690,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.9730789125811827E-2"/>
+                  <c:y val="0.21336663497928363"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -727,378 +728,648 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'FrequencyDrift2021-07-21trail3'!$A$9:$A$68</c:f>
+              <c:f>'FrequencyDrift2021-07-22trial7'!$A$7:$A$111</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="105"/>
                 <c:pt idx="0">
-                  <c:v>2.41</c:v>
+                  <c:v>2.3260000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.721</c:v>
+                  <c:v>17.646999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.067</c:v>
+                  <c:v>32.982999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.398000000000003</c:v>
+                  <c:v>48.308999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.728000000000002</c:v>
+                  <c:v>63.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79.054000000000002</c:v>
+                  <c:v>78.944999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94.376999999999995</c:v>
+                  <c:v>94.292000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>109.703</c:v>
+                  <c:v>109.619</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>125.036</c:v>
+                  <c:v>124.95399999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>140.364</c:v>
+                  <c:v>140.292</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>155.69200000000001</c:v>
+                  <c:v>155.62700000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>171.023</c:v>
+                  <c:v>170.941</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>186.346</c:v>
+                  <c:v>186.291</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>201.673</c:v>
+                  <c:v>201.61600000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>217.00700000000001</c:v>
+                  <c:v>216.953</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>232.327</c:v>
+                  <c:v>232.29300000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>247.66</c:v>
+                  <c:v>247.613</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>262.995</c:v>
+                  <c:v>262.94</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>278.32299999999998</c:v>
+                  <c:v>278.286</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>293.65100000000001</c:v>
+                  <c:v>293.61700000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>308.97800000000001</c:v>
+                  <c:v>308.947</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>324.30500000000001</c:v>
+                  <c:v>324.291</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>339.63499999999999</c:v>
+                  <c:v>339.62</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>355.00200000000001</c:v>
+                  <c:v>354.94499999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>370.31799999999998</c:v>
+                  <c:v>370.30099999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>385.654</c:v>
+                  <c:v>385.63600000000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>400.98200000000003</c:v>
+                  <c:v>401.00299999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>416.31099999999998</c:v>
+                  <c:v>416.32900000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>431.64600000000002</c:v>
+                  <c:v>431.65699999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>446.976</c:v>
+                  <c:v>447.03</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>462.29399999999998</c:v>
+                  <c:v>462.37099999999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>477.63799999999998</c:v>
+                  <c:v>477.69799999999998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>492.96600000000001</c:v>
+                  <c:v>493.02499999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>508.29700000000003</c:v>
+                  <c:v>508.35</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>523.61300000000006</c:v>
+                  <c:v>523.67700000000002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>538.94100000000003</c:v>
+                  <c:v>539.01900000000001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>554.28</c:v>
+                  <c:v>554.33900000000006</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>569.62599999999998</c:v>
+                  <c:v>569.68600000000004</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>584.95500000000004</c:v>
+                  <c:v>585.02</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>600.26900000000001</c:v>
+                  <c:v>600.34900000000005</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>615.61199999999997</c:v>
+                  <c:v>615.66999999999996</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>630.92399999999998</c:v>
+                  <c:v>631.01700000000005</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>646.28200000000004</c:v>
+                  <c:v>646.34299999999996</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>661.64200000000005</c:v>
+                  <c:v>661.67</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>676.96699999999998</c:v>
+                  <c:v>677.01499999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>692.29499999999996</c:v>
+                  <c:v>692.34900000000005</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>707.64700000000005</c:v>
+                  <c:v>707.67</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>722.97299999999996</c:v>
+                  <c:v>723.02700000000004</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>738.30600000000004</c:v>
+                  <c:v>738.35699999999997</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>753.625</c:v>
+                  <c:v>753.697</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>768.952</c:v>
+                  <c:v>769.03899999999999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>784.28200000000004</c:v>
+                  <c:v>784.36</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>799.60799999999995</c:v>
+                  <c:v>799.69600000000003</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>814.94200000000001</c:v>
+                  <c:v>815.02099999999996</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>830.274</c:v>
+                  <c:v>830.35699999999997</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>845.59500000000003</c:v>
+                  <c:v>845.68299999999999</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>860.91899999999998</c:v>
+                  <c:v>861.01599999999996</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>876.25300000000004</c:v>
+                  <c:v>876.34299999999996</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>891.57799999999997</c:v>
+                  <c:v>891.66499999999996</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>906.90800000000002</c:v>
+                  <c:v>907.01599999999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>922.34299999999996</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>937.67600000000004</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>953.01499999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>968.34699999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>983.67399999999998</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>999.02099999999996</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1014.347</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1029.673</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1045.019</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1060.366</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1075.6890000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1091.0170000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1106.3440000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1121.662</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1137.0170000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1152.366</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1167.694</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1183.0229999999999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1198.3620000000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1213.7429999999999</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1229.069</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1244.395</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1259.7439999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1275.0740000000001</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1290.422</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1305.751</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1321.0719999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1336.4059999999999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1351.7280000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1367.0419999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1382.3610000000001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1397.694</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1413.021</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1428.3630000000001</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1443.6869999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1459.0360000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1474.364</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1489.69</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1505.0229999999999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1520.3409999999999</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1535.662</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1551.011</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1566.326</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1581.6769999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1597.0139999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'FrequencyDrift2021-07-21trail3'!$B$9:$B$68</c:f>
+              <c:f>'FrequencyDrift2021-07-22trial7'!$B$7:$B$111</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="105"/>
                 <c:pt idx="0">
-                  <c:v>-5.7346780945888103E-4</c:v>
+                  <c:v>-7.9433838129066101E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.1469356189177599E-3</c:v>
+                  <c:v>-2.3362893567372401E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9115593648629301E-4</c:v>
+                  <c:v>-1.8690314853897899E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.67618311080811E-3</c:v>
+                  <c:v>-1.40177361404234E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0584949837806899E-3</c:v>
+                  <c:v>-9.3451574269489595E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2938712378355198E-3</c:v>
+                  <c:v>-6.5416101988642703E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6319627932395798E-3</c:v>
+                  <c:v>-4.6725787134744802E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4850271743218099E-3</c:v>
+                  <c:v>-7.4761259415591702E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0584949837806899E-3</c:v>
+                  <c:v>-5.1398365848219297E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4408068567532801E-3</c:v>
+                  <c:v>-7.0088680702117198E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.5877424756710396E-3</c:v>
+                  <c:v>-4.6725787134744802E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.5877424756710396E-3</c:v>
+                  <c:v>-7.0088680702117198E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.1612102851299304E-3</c:v>
+                  <c:v>-2.80354722808468E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.3081459040476903E-3</c:v>
+                  <c:v>-1.02796731696438E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.2639255864791596E-3</c:v>
+                  <c:v>-2.80354722808468E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.6904577770202697E-3</c:v>
+                  <c:v>-8.8778995556015108E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.4108612053969203E-3</c:v>
+                  <c:v>-6.5416101988642703E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.60201714188321E-3</c:v>
+                  <c:v>-7.9433838129066101E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.9401086972872692E-3</c:v>
+                  <c:v>-7.9433838129066101E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.2042823998636499E-2</c:v>
+                  <c:v>-5.6070944561693696E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.1660512125663901E-2</c:v>
+                  <c:v>-7.4761259415591702E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.08958883797187E-2</c:v>
+                  <c:v>-9.3451574269489603E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.1851668062150199E-2</c:v>
+                  <c:v>-8.8778995556015108E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.1469356189177601E-2</c:v>
+                  <c:v>-7.0088680702117198E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.2042823998636499E-2</c:v>
+                  <c:v>-6.07435232751682E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2998603681067899E-2</c:v>
+                  <c:v>-6.07435232751682E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.45278511729583E-2</c:v>
+                  <c:v>-4.6725787134744802E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.47190071094446E-2</c:v>
+                  <c:v>-2.80354722808468E-3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.6057098664848599E-2</c:v>
+                  <c:v>-4.2053208421270298E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.81598139661979E-2</c:v>
+                  <c:v>-9.8124152982964098E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.81598139661979E-2</c:v>
+                  <c:v>-6.07435232751682E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.77775020932253E-2</c:v>
+                  <c:v>-4.6725787134744802E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.94979055216019E-2</c:v>
+                  <c:v>-7.9433838129066101E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.91155936486293E-2</c:v>
+                  <c:v>-8.8778995556015108E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.91155936486293E-2</c:v>
+                  <c:v>-2.3362893567372401E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.98802173945745E-2</c:v>
+                  <c:v>-3.7380629707795799E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.1791776759437401E-2</c:v>
+                  <c:v>-6.07435232751682E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.1027153013492301E-2</c:v>
+                  <c:v>-7.4761259415591702E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.3321024251327802E-2</c:v>
+                  <c:v>-5.6070944561693696E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.2938712378355201E-2</c:v>
+                  <c:v>-8.8778995556015108E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.3129868314841501E-2</c:v>
+                  <c:v>-6.07435232751682E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.3894492060786698E-2</c:v>
+                  <c:v>-8.8778995556015108E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.3129868314841501E-2</c:v>
+                  <c:v>-7.4761259415591702E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.2747556441868901E-2</c:v>
+                  <c:v>-6.5416101988642703E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.4467959870245502E-2</c:v>
+                  <c:v>-7.4761259415591702E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.2938712378355201E-2</c:v>
+                  <c:v>-4.2053208421270298E-3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.5232583616190699E-2</c:v>
+                  <c:v>-4.6725787134744802E-3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.5232583616190699E-2</c:v>
+                  <c:v>-4.6725787134744802E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.6188363298622199E-2</c:v>
+                  <c:v>-6.5416101988642703E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.5423739552676999E-2</c:v>
+                  <c:v>-7.0088680702117198E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.4085647997272999E-2</c:v>
+                  <c:v>-5.1398365848219297E-3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.4659115806731802E-2</c:v>
+                  <c:v>4.6725787134744797E-4</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.5041427679704398E-2</c:v>
+                  <c:v>-3.27080509943213E-3</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.5806051425649599E-2</c:v>
+                  <c:v>-4.2053208421270298E-3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.5614895489163299E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.5423739552676999E-2</c:v>
+                  <c:v>6.07435232751682E-3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.4276803933759201E-2</c:v>
+                  <c:v>-3.27080509943213E-3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.5041427679704398E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.5614895489163299E-2</c:v>
+                  <c:v>-4.2053208421270298E-3</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.3894492060786698E-2</c:v>
+                  <c:v>3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-1.8690314853897899E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.3362893567372401E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.2053208421270298E-3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.80354722808468E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-3.27080509943213E-3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.3362893567372401E-3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-3.27080509943213E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.2053208421270298E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-1.8690314853897899E-3</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-1.40177361404234E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.80354722808468E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.1398365848219297E-3</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.6725787134744797E-4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.1398365848219297E-3</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.80354722808468E-3</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.80354722808468E-3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.1398365848219297E-3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.1398365848219297E-3</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.6725787134744797E-4</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.3362893567372401E-3</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.80354722808468E-3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.3362893567372401E-3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.6070944561693696E-3</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.80354722808468E-3</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.3362893567372401E-3</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.07435232751682E-3</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.3362893567372401E-3</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4.6725787134744797E-4</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.6725787134744797E-4</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.6725787134744797E-4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.6070944561693696E-3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.27080509943213E-3</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5.1398365848219297E-3</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>4.6725787134744802E-3</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>8.8778995556015108E-3</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.07469310409913E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3.27080509943213E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1106,7 +1377,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8132-524B-9611-85A0442CE8A9}"/>
+              <c16:uniqueId val="{00000000-9E3A-6447-A7C5-829154A0FDC2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1118,11 +1389,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1787022720"/>
-        <c:axId val="1787024368"/>
+        <c:axId val="1630477296"/>
+        <c:axId val="1630478944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1787022720"/>
+        <c:axId val="1630477296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,12 +1450,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1787024368"/>
+        <c:crossAx val="1630478944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1787024368"/>
+        <c:axId val="1630478944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1512,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1787022720"/>
+        <c:crossAx val="1630477296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1857,23 +2128,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E222D28A-BB9D-D14A-B7F0-D6B289117DCE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99EDFD10-A579-A54D-957E-70357D4142DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2191,739 +2462,2586 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B68"/>
+    <sheetView tabSelected="1" topLeftCell="E153" zoomScale="117" workbookViewId="0">
+      <selection activeCell="R171" sqref="R171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>128.27000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>4.6619999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2.3260000000000001</v>
       </c>
       <c r="B7">
+        <v>-7.9433838129066101E-3</v>
+      </c>
+      <c r="C7">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D7">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>17.646999999999998</v>
+      </c>
+      <c r="B8">
+        <v>-2.3362893567372401E-3</v>
+      </c>
+      <c r="C8">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D8">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>32.982999999999997</v>
+      </c>
+      <c r="B9">
+        <v>-1.8690314853897899E-3</v>
+      </c>
+      <c r="C9">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D9">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>48.308999999999997</v>
+      </c>
+      <c r="B10">
+        <v>-1.40177361404234E-3</v>
+      </c>
+      <c r="C10">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D10">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>63.625</v>
+      </c>
+      <c r="B11">
+        <v>-9.3451574269489595E-4</v>
+      </c>
+      <c r="C11">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D11">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>78.944999999999993</v>
+      </c>
+      <c r="B12">
+        <v>-6.5416101988642703E-3</v>
+      </c>
+      <c r="C12">
+        <v>127.662602965403</v>
+      </c>
+      <c r="D12">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>94.292000000000002</v>
+      </c>
+      <c r="B13">
+        <v>-4.6725787134744802E-3</v>
+      </c>
+      <c r="C13">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D13">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>109.619</v>
+      </c>
+      <c r="B14">
+        <v>-7.4761259415591702E-3</v>
+      </c>
+      <c r="C14">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D14">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>124.95399999999999</v>
+      </c>
+      <c r="B15">
+        <v>-5.1398365848219297E-3</v>
+      </c>
+      <c r="C15">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D15">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>140.292</v>
+      </c>
+      <c r="B16">
+        <v>-7.0088680702117198E-3</v>
+      </c>
+      <c r="C16">
+        <v>127.662602965403</v>
+      </c>
+      <c r="D16">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>155.62700000000001</v>
+      </c>
+      <c r="B17">
+        <v>-4.6725787134744802E-3</v>
+      </c>
+      <c r="C17">
+        <v>127.65416803953801</v>
+      </c>
+      <c r="D17">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>170.941</v>
+      </c>
+      <c r="B18">
+        <v>-7.0088680702117198E-3</v>
+      </c>
+      <c r="C18">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D18">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>186.291</v>
+      </c>
+      <c r="B19">
+        <v>-2.80354722808468E-3</v>
+      </c>
+      <c r="C19">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D19">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>201.61600000000001</v>
+      </c>
+      <c r="B20">
+        <v>-1.02796731696438E-2</v>
+      </c>
+      <c r="C20">
+        <v>127.662602965403</v>
+      </c>
+      <c r="D20">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>216.953</v>
+      </c>
+      <c r="B21">
+        <v>-2.80354722808468E-3</v>
+      </c>
+      <c r="C21">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D21">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>232.29300000000001</v>
+      </c>
+      <c r="B22">
+        <v>-8.8778995556015108E-3</v>
+      </c>
+      <c r="C22">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D22">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>247.613</v>
+      </c>
+      <c r="B23">
+        <v>-6.5416101988642703E-3</v>
+      </c>
+      <c r="C23">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D23">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>262.94</v>
+      </c>
+      <c r="B24">
+        <v>-7.9433838129066101E-3</v>
+      </c>
+      <c r="C24">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D24">
+        <v>64.5550537109375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>278.286</v>
+      </c>
+      <c r="B25">
+        <v>-7.9433838129066101E-3</v>
+      </c>
+      <c r="C25">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D25">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>293.61700000000002</v>
+      </c>
+      <c r="B26">
+        <v>-5.6070944561693696E-3</v>
+      </c>
+      <c r="C26">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D26">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>308.947</v>
+      </c>
+      <c r="B27">
+        <v>-7.4761259415591702E-3</v>
+      </c>
+      <c r="C27">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D27">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>324.291</v>
+      </c>
+      <c r="B28">
+        <v>-9.3451574269489603E-3</v>
+      </c>
+      <c r="C28">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D28">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>339.62</v>
+      </c>
+      <c r="B29">
+        <v>-8.8778995556015108E-3</v>
+      </c>
+      <c r="C29">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D29">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>354.94499999999999</v>
+      </c>
+      <c r="B30">
+        <v>-7.0088680702117198E-3</v>
+      </c>
+      <c r="C30">
+        <v>127.65416803953801</v>
+      </c>
+      <c r="D30">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>370.30099999999999</v>
+      </c>
+      <c r="B31">
+        <v>-6.07435232751682E-3</v>
+      </c>
+      <c r="C31">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D31">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>385.63600000000002</v>
+      </c>
+      <c r="B32">
+        <v>-6.07435232751682E-3</v>
+      </c>
+      <c r="C32">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D32">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>401.00299999999999</v>
+      </c>
+      <c r="B33">
+        <v>-4.6725787134744802E-3</v>
+      </c>
+      <c r="C33">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D33">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>416.32900000000001</v>
+      </c>
+      <c r="B34">
+        <v>-2.80354722808468E-3</v>
+      </c>
+      <c r="C34">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D34">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>431.65699999999998</v>
+      </c>
+      <c r="B35">
+        <v>-4.2053208421270298E-3</v>
+      </c>
+      <c r="C35">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D35">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>447.03</v>
+      </c>
+      <c r="B36">
+        <v>-9.8124152982964098E-3</v>
+      </c>
+      <c r="C36">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D36">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>462.37099999999998</v>
+      </c>
+      <c r="B37">
+        <v>-6.07435232751682E-3</v>
+      </c>
+      <c r="C37">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D37">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>477.69799999999998</v>
+      </c>
+      <c r="B38">
+        <v>-4.6725787134744802E-3</v>
+      </c>
+      <c r="C38">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D38">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>493.02499999999998</v>
+      </c>
+      <c r="B39">
+        <v>-7.9433838129066101E-3</v>
+      </c>
+      <c r="C39">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D39">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>508.35</v>
+      </c>
+      <c r="B40">
+        <v>-8.8778995556015108E-3</v>
+      </c>
+      <c r="C40">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D40">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>523.67700000000002</v>
+      </c>
+      <c r="B41">
+        <v>-2.3362893567372401E-3</v>
+      </c>
+      <c r="C41">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D41">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>539.01900000000001</v>
+      </c>
+      <c r="B42">
+        <v>-3.7380629707795799E-3</v>
+      </c>
+      <c r="C42">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D42">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>554.33900000000006</v>
+      </c>
+      <c r="B43">
+        <v>-6.07435232751682E-3</v>
+      </c>
+      <c r="C43">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D43">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>569.68600000000004</v>
+      </c>
+      <c r="B44">
+        <v>-7.4761259415591702E-3</v>
+      </c>
+      <c r="C44">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D44">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>585.02</v>
+      </c>
+      <c r="B45">
+        <v>-5.6070944561693696E-3</v>
+      </c>
+      <c r="C45">
+        <v>127.721647446457</v>
+      </c>
+      <c r="D45">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>600.34900000000005</v>
+      </c>
+      <c r="B46">
+        <v>-8.8778995556015108E-3</v>
+      </c>
+      <c r="C46">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D46">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>615.66999999999996</v>
+      </c>
+      <c r="B47">
+        <v>-6.07435232751682E-3</v>
+      </c>
+      <c r="C47">
+        <v>127.65416803953801</v>
+      </c>
+      <c r="D47">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>631.01700000000005</v>
+      </c>
+      <c r="B48">
+        <v>-8.8778995556015108E-3</v>
+      </c>
+      <c r="C48">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D48">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>646.34299999999996</v>
+      </c>
+      <c r="B49">
+        <v>-7.4761259415591702E-3</v>
+      </c>
+      <c r="C49">
+        <v>127.65416803953801</v>
+      </c>
+      <c r="D49">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>661.67</v>
+      </c>
+      <c r="B50">
+        <v>-6.5416101988642703E-3</v>
+      </c>
+      <c r="C50">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D50">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>677.01499999999999</v>
+      </c>
+      <c r="B51">
+        <v>-7.4761259415591702E-3</v>
+      </c>
+      <c r="C51">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D51">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>692.34900000000005</v>
+      </c>
+      <c r="B52">
+        <v>-4.2053208421270298E-3</v>
+      </c>
+      <c r="C52">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D52">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>707.67</v>
+      </c>
+      <c r="B53">
+        <v>-4.6725787134744802E-3</v>
+      </c>
+      <c r="C53">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D53">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>723.02700000000004</v>
+      </c>
+      <c r="B54">
+        <v>-4.6725787134744802E-3</v>
+      </c>
+      <c r="C54">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D54">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>738.35699999999997</v>
+      </c>
+      <c r="B55">
+        <v>-6.5416101988642703E-3</v>
+      </c>
+      <c r="C55">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D55">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>753.697</v>
+      </c>
+      <c r="B56">
+        <v>-7.0088680702117198E-3</v>
+      </c>
+      <c r="C56">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D56">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>769.03899999999999</v>
+      </c>
+      <c r="B57">
+        <v>-5.1398365848219297E-3</v>
+      </c>
+      <c r="C57">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D57">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>784.36</v>
+      </c>
+      <c r="B58">
+        <v>4.6725787134744797E-4</v>
+      </c>
+      <c r="C58">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D58">
+        <v>64.537353515625</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>799.69600000000003</v>
+      </c>
+      <c r="B59">
+        <v>-3.27080509943213E-3</v>
+      </c>
+      <c r="C59">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D59">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>815.02099999999996</v>
+      </c>
+      <c r="B60">
+        <v>-4.2053208421270298E-3</v>
+      </c>
+      <c r="C60">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D60">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>830.35699999999997</v>
+      </c>
+      <c r="B61">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2.41</v>
-      </c>
-      <c r="B9">
-        <v>-5.7346780945888103E-4</v>
-      </c>
-      <c r="C9">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>17.721</v>
-      </c>
-      <c r="B10">
-        <v>-1.1469356189177599E-3</v>
-      </c>
-      <c r="C10">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>33.067</v>
-      </c>
-      <c r="B11">
-        <v>1.9115593648629301E-4</v>
-      </c>
-      <c r="C11">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>48.398000000000003</v>
-      </c>
-      <c r="B12">
-        <v>2.67618311080811E-3</v>
-      </c>
-      <c r="C12">
-        <v>128.177133443163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>63.728000000000002</v>
-      </c>
-      <c r="B13">
-        <v>3.0584949837806899E-3</v>
-      </c>
-      <c r="C13">
-        <v>128.177133443163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>79.054000000000002</v>
-      </c>
-      <c r="B14">
-        <v>2.2938712378355198E-3</v>
-      </c>
-      <c r="C14">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>94.376999999999995</v>
-      </c>
-      <c r="B15">
-        <v>3.6319627932395798E-3</v>
-      </c>
-      <c r="C15">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>109.703</v>
-      </c>
-      <c r="B16">
-        <v>2.4850271743218099E-3</v>
-      </c>
-      <c r="C16">
-        <v>128.18556836902701</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>125.036</v>
-      </c>
-      <c r="B17">
-        <v>3.0584949837806899E-3</v>
-      </c>
-      <c r="C17">
-        <v>128.185568369028</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>140.364</v>
-      </c>
-      <c r="B18">
-        <v>3.4408068567532801E-3</v>
-      </c>
-      <c r="C18">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>155.69200000000001</v>
-      </c>
-      <c r="B19">
-        <v>4.5877424756710396E-3</v>
-      </c>
-      <c r="C19">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>171.023</v>
-      </c>
-      <c r="B20">
-        <v>4.5877424756710396E-3</v>
-      </c>
-      <c r="C20">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>186.346</v>
-      </c>
-      <c r="B21">
-        <v>5.1612102851299304E-3</v>
-      </c>
-      <c r="C21">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>201.673</v>
-      </c>
-      <c r="B22">
-        <v>6.3081459040476903E-3</v>
-      </c>
-      <c r="C22">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>217.00700000000001</v>
-      </c>
-      <c r="B23">
-        <v>7.2639255864791596E-3</v>
-      </c>
-      <c r="C23">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>232.327</v>
-      </c>
-      <c r="B24">
-        <v>6.6904577770202697E-3</v>
-      </c>
-      <c r="C24">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>247.66</v>
-      </c>
-      <c r="B25">
-        <v>8.4108612053969203E-3</v>
-      </c>
-      <c r="C25">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>262.995</v>
-      </c>
-      <c r="B26">
-        <v>8.60201714188321E-3</v>
-      </c>
-      <c r="C26">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>278.32299999999998</v>
-      </c>
-      <c r="B27">
-        <v>9.9401086972872692E-3</v>
-      </c>
-      <c r="C27">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>293.65100000000001</v>
-      </c>
-      <c r="B28">
-        <v>1.2042823998636499E-2</v>
-      </c>
-      <c r="C28">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>308.97800000000001</v>
-      </c>
-      <c r="B29">
-        <v>1.1660512125663901E-2</v>
-      </c>
-      <c r="C29">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>324.30500000000001</v>
-      </c>
-      <c r="B30">
-        <v>1.08958883797187E-2</v>
-      </c>
-      <c r="C30">
-        <v>128.227742998352</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>339.63499999999999</v>
-      </c>
-      <c r="B31">
-        <v>1.1851668062150199E-2</v>
-      </c>
-      <c r="C31">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>355.00200000000001</v>
-      </c>
-      <c r="B32">
-        <v>1.1469356189177601E-2</v>
-      </c>
-      <c r="C32">
-        <v>128.185568369028</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>370.31799999999998</v>
-      </c>
-      <c r="B33">
-        <v>1.2042823998636499E-2</v>
-      </c>
-      <c r="C33">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>385.654</v>
-      </c>
-      <c r="B34">
-        <v>1.2998603681067899E-2</v>
-      </c>
-      <c r="C34">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>400.98200000000003</v>
-      </c>
-      <c r="B35">
-        <v>1.45278511729583E-2</v>
-      </c>
-      <c r="C35">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>416.31099999999998</v>
-      </c>
-      <c r="B36">
-        <v>1.47190071094446E-2</v>
-      </c>
-      <c r="C36">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>431.64600000000002</v>
-      </c>
-      <c r="B37">
-        <v>1.6057098664848599E-2</v>
-      </c>
-      <c r="C37">
-        <v>128.20243822075699</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>446.976</v>
-      </c>
-      <c r="B38">
-        <v>1.81598139661979E-2</v>
-      </c>
-      <c r="C38">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>462.29399999999998</v>
-      </c>
-      <c r="B39">
-        <v>1.81598139661979E-2</v>
-      </c>
-      <c r="C39">
-        <v>128.236177924217</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>477.63799999999998</v>
-      </c>
-      <c r="B40">
-        <v>1.77775020932253E-2</v>
-      </c>
-      <c r="C40">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>492.96600000000001</v>
-      </c>
-      <c r="B41">
-        <v>1.94979055216019E-2</v>
-      </c>
-      <c r="C41">
-        <v>128.20243822075699</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>508.29700000000003</v>
-      </c>
-      <c r="B42">
-        <v>1.91155936486293E-2</v>
-      </c>
-      <c r="C42">
-        <v>128.236177924217</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>523.61300000000006</v>
-      </c>
-      <c r="B43">
-        <v>1.91155936486293E-2</v>
-      </c>
-      <c r="C43">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>538.94100000000003</v>
-      </c>
-      <c r="B44">
-        <v>1.98802173945745E-2</v>
-      </c>
-      <c r="C44">
-        <v>128.20243822075699</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>554.28</v>
-      </c>
-      <c r="B45">
-        <v>2.1791776759437401E-2</v>
-      </c>
-      <c r="C45">
-        <v>128.185568369028</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>569.62599999999998</v>
-      </c>
-      <c r="B46">
-        <v>2.1027153013492301E-2</v>
-      </c>
-      <c r="C46">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>584.95500000000004</v>
-      </c>
-      <c r="B47">
-        <v>2.3321024251327802E-2</v>
-      </c>
-      <c r="C47">
-        <v>128.227742998352</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>600.26900000000001</v>
-      </c>
-      <c r="B48">
-        <v>2.2938712378355201E-2</v>
-      </c>
-      <c r="C48">
-        <v>128.227742998352</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>615.61199999999997</v>
-      </c>
-      <c r="B49">
-        <v>2.3129868314841501E-2</v>
-      </c>
-      <c r="C49">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>630.92399999999998</v>
-      </c>
-      <c r="B50">
-        <v>2.3894492060786698E-2</v>
-      </c>
-      <c r="C50">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>646.28200000000004</v>
-      </c>
-      <c r="B51">
-        <v>2.3129868314841501E-2</v>
-      </c>
-      <c r="C51">
-        <v>128.24461285008201</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>661.64200000000005</v>
-      </c>
-      <c r="B52">
-        <v>2.2747556441868901E-2</v>
-      </c>
-      <c r="C52">
-        <v>128.227742998352</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>676.96699999999998</v>
-      </c>
-      <c r="B53">
-        <v>2.4467959870245502E-2</v>
-      </c>
-      <c r="C53">
-        <v>128.19400329489201</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>692.29499999999996</v>
-      </c>
-      <c r="B54">
-        <v>2.2938712378355201E-2</v>
-      </c>
-      <c r="C54">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>707.64700000000005</v>
-      </c>
-      <c r="B55">
-        <v>2.5232583616190699E-2</v>
-      </c>
-      <c r="C55">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>722.97299999999996</v>
-      </c>
-      <c r="B56">
-        <v>2.5232583616190699E-2</v>
-      </c>
-      <c r="C56">
-        <v>128.24461285008201</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>738.30600000000004</v>
-      </c>
-      <c r="B57">
-        <v>2.6188363298622199E-2</v>
-      </c>
-      <c r="C57">
-        <v>128.25304777594701</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>753.625</v>
-      </c>
-      <c r="B58">
-        <v>2.5423739552676999E-2</v>
-      </c>
-      <c r="C58">
-        <v>128.24461285008201</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>768.952</v>
-      </c>
-      <c r="B59">
-        <v>2.4085647997272999E-2</v>
-      </c>
-      <c r="C59">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>784.28200000000004</v>
-      </c>
-      <c r="B60">
-        <v>2.4659115806731802E-2</v>
-      </c>
-      <c r="C60">
-        <v>128.227742998352</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>799.60799999999995</v>
-      </c>
-      <c r="B61">
-        <v>2.5041427679704398E-2</v>
-      </c>
       <c r="C61">
-        <v>128.24461285008201</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D61">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>814.94200000000001</v>
+        <v>845.68299999999999</v>
       </c>
       <c r="B62">
-        <v>2.5806051425649599E-2</v>
+        <v>6.07435232751682E-3</v>
       </c>
       <c r="C62">
-        <v>128.236177924217</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D62">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>830.274</v>
+        <v>861.01599999999996</v>
       </c>
       <c r="B63">
-        <v>2.5614895489163299E-2</v>
+        <v>-3.27080509943213E-3</v>
       </c>
       <c r="C63">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D63">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>845.59500000000003</v>
+        <v>876.34299999999996</v>
       </c>
       <c r="B64">
-        <v>2.5423739552676999E-2</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>128.21087314662199</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D64">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>860.91899999999998</v>
+        <v>891.66499999999996</v>
       </c>
       <c r="B65">
-        <v>2.4276803933759201E-2</v>
+        <v>-4.2053208421270298E-3</v>
       </c>
       <c r="C65">
-        <v>128.236177924217</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D65">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>876.25300000000004</v>
+        <v>907.01599999999996</v>
       </c>
       <c r="B66">
-        <v>2.5041427679704398E-2</v>
+        <v>3.7380629707795799E-3</v>
       </c>
       <c r="C66">
-        <v>128.219308072487</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D66">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>891.57799999999997</v>
+        <v>922.34299999999996</v>
       </c>
       <c r="B67">
-        <v>2.5614895489163299E-2</v>
+        <v>3.7380629707795799E-3</v>
       </c>
       <c r="C67">
-        <v>128.227742998352</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D67">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>906.90800000000002</v>
+        <v>937.67600000000004</v>
       </c>
       <c r="B68">
-        <v>2.3894492060786698E-2</v>
+        <v>-1.8690314853897899E-3</v>
       </c>
       <c r="C68">
-        <v>128.219308072487</v>
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D68">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>953.01499999999999</v>
+      </c>
+      <c r="B69">
+        <v>2.3362893567372401E-3</v>
+      </c>
+      <c r="C69">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D69">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>968.34699999999998</v>
+      </c>
+      <c r="B70">
+        <v>-3.7380629707795799E-3</v>
+      </c>
+      <c r="C70">
+        <v>127.72164744645799</v>
+      </c>
+      <c r="D70">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>983.67399999999998</v>
+      </c>
+      <c r="B71">
+        <v>4.2053208421270298E-3</v>
+      </c>
+      <c r="C71">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D71">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>999.02099999999996</v>
+      </c>
+      <c r="B72">
+        <v>2.80354722808468E-3</v>
+      </c>
+      <c r="C72">
+        <v>127.72164744645799</v>
+      </c>
+      <c r="D72">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>1014.347</v>
+      </c>
+      <c r="B73">
+        <v>-3.27080509943213E-3</v>
+      </c>
+      <c r="C73">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D73">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1029.673</v>
+      </c>
+      <c r="B74">
+        <v>2.3362893567372401E-3</v>
+      </c>
+      <c r="C74">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D74">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>1045.019</v>
+      </c>
+      <c r="B75">
+        <v>-3.27080509943213E-3</v>
+      </c>
+      <c r="C75">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D75">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>1060.366</v>
+      </c>
+      <c r="B76">
+        <v>4.2053208421270298E-3</v>
+      </c>
+      <c r="C76">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D76">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>1075.6890000000001</v>
+      </c>
+      <c r="B77">
+        <v>-1.8690314853897899E-3</v>
+      </c>
+      <c r="C77">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D77">
+        <v>64.5196533203125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>1091.0170000000001</v>
+      </c>
+      <c r="B78">
+        <v>-1.40177361404234E-3</v>
+      </c>
+      <c r="C78">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D78">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>1106.3440000000001</v>
+      </c>
+      <c r="B79">
+        <v>2.80354722808468E-3</v>
+      </c>
+      <c r="C79">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D79">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>1121.662</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D80">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1137.0170000000001</v>
+      </c>
+      <c r="B81">
+        <v>5.1398365848219297E-3</v>
+      </c>
+      <c r="C81">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D81">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>1152.366</v>
+      </c>
+      <c r="B82">
+        <v>4.6725787134744797E-4</v>
+      </c>
+      <c r="C82">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D82">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1167.694</v>
+      </c>
+      <c r="B83">
+        <v>5.1398365848219297E-3</v>
+      </c>
+      <c r="C83">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D83">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1183.0229999999999</v>
+      </c>
+      <c r="B84">
+        <v>2.80354722808468E-3</v>
+      </c>
+      <c r="C84">
+        <v>127.679472817133</v>
+      </c>
+      <c r="D84">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1198.3620000000001</v>
+      </c>
+      <c r="B85">
+        <v>3.7380629707795799E-3</v>
+      </c>
+      <c r="C85">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D85">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1213.7429999999999</v>
+      </c>
+      <c r="B86">
+        <v>2.80354722808468E-3</v>
+      </c>
+      <c r="C86">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D86">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1229.069</v>
+      </c>
+      <c r="B87">
+        <v>5.1398365848219297E-3</v>
+      </c>
+      <c r="C87">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D87">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1244.395</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>127.72164744645799</v>
+      </c>
+      <c r="D88">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1259.7439999999999</v>
+      </c>
+      <c r="B89">
+        <v>5.1398365848219297E-3</v>
+      </c>
+      <c r="C89">
+        <v>127.671037891268</v>
+      </c>
+      <c r="D89">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1275.0740000000001</v>
+      </c>
+      <c r="B90">
+        <v>4.6725787134744797E-4</v>
+      </c>
+      <c r="C90">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D90">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1290.422</v>
+      </c>
+      <c r="B91">
+        <v>2.3362893567372401E-3</v>
+      </c>
+      <c r="C91">
+        <v>127.72164744645799</v>
+      </c>
+      <c r="D91">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1305.751</v>
+      </c>
+      <c r="B92">
+        <v>2.80354722808468E-3</v>
+      </c>
+      <c r="C92">
+        <v>127.72164744645799</v>
+      </c>
+      <c r="D92">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1321.0719999999999</v>
+      </c>
+      <c r="B93">
+        <v>2.3362893567372401E-3</v>
+      </c>
+      <c r="C93">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D93">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1336.4059999999999</v>
+      </c>
+      <c r="B94">
+        <v>5.6070944561693696E-3</v>
+      </c>
+      <c r="C94">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D94">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1351.7280000000001</v>
+      </c>
+      <c r="B95">
+        <v>2.80354722808468E-3</v>
+      </c>
+      <c r="C95">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D95">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1367.0419999999999</v>
+      </c>
+      <c r="B96">
+        <v>2.3362893567372401E-3</v>
+      </c>
+      <c r="C96">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D96">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>1382.3610000000001</v>
+      </c>
+      <c r="B97">
+        <v>6.07435232751682E-3</v>
+      </c>
+      <c r="C97">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D97">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>1397.694</v>
+      </c>
+      <c r="B98">
+        <v>2.3362893567372401E-3</v>
+      </c>
+      <c r="C98">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D98">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>1413.021</v>
+      </c>
+      <c r="B99">
+        <v>4.6725787134744797E-4</v>
+      </c>
+      <c r="C99">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D99">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>1428.3630000000001</v>
+      </c>
+      <c r="B100">
+        <v>4.6725787134744797E-4</v>
+      </c>
+      <c r="C100">
+        <v>127.68790774299799</v>
+      </c>
+      <c r="D100">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>1443.6869999999999</v>
+      </c>
+      <c r="B101">
+        <v>4.6725787134744797E-4</v>
+      </c>
+      <c r="C101">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D101">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>1459.0360000000001</v>
+      </c>
+      <c r="B102">
+        <v>5.6070944561693696E-3</v>
+      </c>
+      <c r="C102">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D102">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>1474.364</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>127.721647446457</v>
+      </c>
+      <c r="D103">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>1489.69</v>
+      </c>
+      <c r="B104">
+        <v>3.27080509943213E-3</v>
+      </c>
+      <c r="C104">
+        <v>127.72164744645799</v>
+      </c>
+      <c r="D104">
+        <v>64.501953125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>1505.0229999999999</v>
+      </c>
+      <c r="B105">
+        <v>5.1398365848219297E-3</v>
+      </c>
+      <c r="C105">
+        <v>127.721647446457</v>
+      </c>
+      <c r="D105">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>1520.3409999999999</v>
+      </c>
+      <c r="B106">
+        <v>3.7380629707795799E-3</v>
+      </c>
+      <c r="C106">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D106">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>1535.662</v>
+      </c>
+      <c r="B107">
+        <v>4.6725787134744802E-3</v>
+      </c>
+      <c r="C107">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D107">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>1551.011</v>
+      </c>
+      <c r="B108">
+        <v>8.8778995556015108E-3</v>
+      </c>
+      <c r="C108">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D108">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1566.326</v>
+      </c>
+      <c r="B109">
+        <v>3.7380629707795799E-3</v>
+      </c>
+      <c r="C109">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D109">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>1581.6769999999999</v>
+      </c>
+      <c r="B110">
+        <v>1.07469310409913E-2</v>
+      </c>
+      <c r="C110">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D110">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>1597.0139999999999</v>
+      </c>
+      <c r="B111">
+        <v>3.27080509943213E-3</v>
+      </c>
+      <c r="C111">
+        <v>127.696342668863</v>
+      </c>
+      <c r="D111">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>1612.3320000000001</v>
+      </c>
+      <c r="B112">
+        <v>3.7380629707795799E-3</v>
+      </c>
+      <c r="C112">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D112">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>1627.6510000000001</v>
+      </c>
+      <c r="B113">
+        <v>7.9433838129066101E-3</v>
+      </c>
+      <c r="C113">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D113">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>1642.9780000000001</v>
+      </c>
+      <c r="B114">
+        <v>8.4106416842540596E-3</v>
+      </c>
+      <c r="C114">
+        <v>127.721647446457</v>
+      </c>
+      <c r="D114">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>1658.309</v>
+      </c>
+      <c r="B115">
+        <v>1.21487046550336E-2</v>
+      </c>
+      <c r="C115">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D115">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>1673.627</v>
+      </c>
+      <c r="B116">
+        <v>6.07435232751682E-3</v>
+      </c>
+      <c r="C116">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D116">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>1688.9490000000001</v>
+      </c>
+      <c r="B117">
+        <v>1.1681446783686201E-2</v>
+      </c>
+      <c r="C117">
+        <v>127.721647446457</v>
+      </c>
+      <c r="D117">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>1704.287</v>
+      </c>
+      <c r="B118">
+        <v>8.8778995556015108E-3</v>
+      </c>
+      <c r="C118">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D118">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1719.6220000000001</v>
+      </c>
+      <c r="B119">
+        <v>9.3451574269489603E-3</v>
+      </c>
+      <c r="C119">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D119">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>1734.944</v>
+      </c>
+      <c r="B120">
+        <v>9.3451574269489603E-3</v>
+      </c>
+      <c r="C120">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D120">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>1750.2909999999999</v>
+      </c>
+      <c r="B121">
+        <v>1.3083220397728501E-2</v>
+      </c>
+      <c r="C121">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D121">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1765.615</v>
+      </c>
+      <c r="B122">
+        <v>1.02796731696438E-2</v>
+      </c>
+      <c r="C122">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D122">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>1780.9359999999999</v>
+      </c>
+      <c r="B123">
+        <v>9.8124152982964098E-3</v>
+      </c>
+      <c r="C123">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D123">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>1796.2819999999999</v>
+      </c>
+      <c r="B124">
+        <v>8.4106416842540596E-3</v>
+      </c>
+      <c r="C124">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D124">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>1811.63</v>
+      </c>
+      <c r="B125">
+        <v>1.1681446783686201E-2</v>
+      </c>
+      <c r="C125">
+        <v>127.721647446457</v>
+      </c>
+      <c r="D125">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1826.9480000000001</v>
+      </c>
+      <c r="B126">
+        <v>1.1214188912338699E-2</v>
+      </c>
+      <c r="C126">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D126">
+        <v>64.4842529296875</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>1842.2940000000001</v>
+      </c>
+      <c r="B127">
+        <v>1.5886767625813199E-2</v>
+      </c>
+      <c r="C127">
+        <v>127.713212520593</v>
+      </c>
+      <c r="D127">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>1857.6210000000001</v>
+      </c>
+      <c r="B128">
+        <v>1.2615962526380999E-2</v>
+      </c>
+      <c r="C128">
+        <v>127.704777594728</v>
+      </c>
+      <c r="D128">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1872.954</v>
+      </c>
+      <c r="B129">
+        <v>9.8124152982964098E-3</v>
+      </c>
+      <c r="C129">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D129">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1888.287</v>
+      </c>
+      <c r="B130">
+        <v>1.35504782690759E-2</v>
+      </c>
+      <c r="C130">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D130">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>1903.61</v>
+      </c>
+      <c r="B131">
+        <v>1.49522518831183E-2</v>
+      </c>
+      <c r="C131">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D131">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>1918.943</v>
+      </c>
+      <c r="B132">
+        <v>1.7288541239855501E-2</v>
+      </c>
+      <c r="C132">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D132">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>1934.296</v>
+      </c>
+      <c r="B133">
+        <v>1.21487046550336E-2</v>
+      </c>
+      <c r="C133">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D133">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>1949.626</v>
+      </c>
+      <c r="B134">
+        <v>1.2615962526380999E-2</v>
+      </c>
+      <c r="C134">
+        <v>127.72164744645799</v>
+      </c>
+      <c r="D134">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>1964.961</v>
+      </c>
+      <c r="B135">
+        <v>1.40177361404234E-2</v>
+      </c>
+      <c r="C135">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D135">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>1980.2950000000001</v>
+      </c>
+      <c r="B136">
+        <v>1.49522518831183E-2</v>
+      </c>
+      <c r="C136">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D136">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>1995.615</v>
+      </c>
+      <c r="B137">
+        <v>1.4484994011770801E-2</v>
+      </c>
+      <c r="C137">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D137">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>2010.934</v>
+      </c>
+      <c r="B138">
+        <v>1.82230569825504E-2</v>
+      </c>
+      <c r="C138">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D138">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>2026.2829999999999</v>
+      </c>
+      <c r="B139">
+        <v>1.54195097544657E-2</v>
+      </c>
+      <c r="C139">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D139">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>2041.615</v>
+      </c>
+      <c r="B140">
+        <v>1.3083220397728501E-2</v>
+      </c>
+      <c r="C140">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D140">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>2056.9360000000001</v>
+      </c>
+      <c r="B141">
+        <v>1.7755799111203001E-2</v>
+      </c>
+      <c r="C141">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D141">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>2072.2600000000002</v>
+      </c>
+      <c r="B142">
+        <v>1.40177361404234E-2</v>
+      </c>
+      <c r="C142">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D142">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>2087.587</v>
+      </c>
+      <c r="B143">
+        <v>2.14938620819826E-2</v>
+      </c>
+      <c r="C143">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D143">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>2102.9119999999998</v>
+      </c>
+      <c r="B144">
+        <v>1.5886767625813199E-2</v>
+      </c>
+      <c r="C144">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D144">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>2118.2370000000001</v>
+      </c>
+      <c r="B145">
+        <v>2.2895635696024898E-2</v>
+      </c>
+      <c r="C145">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D145">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>2133.5639999999999</v>
+      </c>
+      <c r="B146">
+        <v>2.5231925052762099E-2</v>
+      </c>
+      <c r="C146">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D146">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>2148.8910000000001</v>
+      </c>
+      <c r="B147">
+        <v>1.7755799111203001E-2</v>
+      </c>
+      <c r="C147">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D147">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>2164.241</v>
+      </c>
+      <c r="B148">
+        <v>1.9624830596592799E-2</v>
+      </c>
+      <c r="C148">
+        <v>127.72164744645799</v>
+      </c>
+      <c r="D148">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>2179.5709999999999</v>
+      </c>
+      <c r="B149">
+        <v>2.6166440795457001E-2</v>
+      </c>
+      <c r="C149">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D149">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>2194.895</v>
+      </c>
+      <c r="B150">
+        <v>1.9624830596592799E-2</v>
+      </c>
+      <c r="C150">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D150">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>2210.2199999999998</v>
+      </c>
+      <c r="B151">
+        <v>2.14938620819826E-2</v>
+      </c>
+      <c r="C151">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D151">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>2225.558</v>
+      </c>
+      <c r="B152">
+        <v>2.1961119953329999E-2</v>
+      </c>
+      <c r="C152">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D152">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>2240.884</v>
+      </c>
+      <c r="B153">
+        <v>2.2895635696024898E-2</v>
+      </c>
+      <c r="C153">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D153">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>2256.2069999999999</v>
+      </c>
+      <c r="B154">
+        <v>2.3362893567372402E-2</v>
+      </c>
+      <c r="C154">
+        <v>127.721647446457</v>
+      </c>
+      <c r="D154">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>2271.5630000000001</v>
+      </c>
+      <c r="B155">
+        <v>2.8969988023541698E-2</v>
+      </c>
+      <c r="C155">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D155">
+        <v>64.466552734375</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>2286.8910000000001</v>
+      </c>
+      <c r="B156">
+        <v>3.1306277380279003E-2</v>
+      </c>
+      <c r="C156">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D156">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>2302.232</v>
+      </c>
+      <c r="B157">
+        <v>2.8035472280846799E-2</v>
+      </c>
+      <c r="C157">
+        <v>127.77225700164701</v>
+      </c>
+      <c r="D157">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>2317.5639999999999</v>
+      </c>
+      <c r="B158">
+        <v>2.3830151438719801E-2</v>
+      </c>
+      <c r="C158">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D158">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>2332.9059999999999</v>
+      </c>
+      <c r="B159">
+        <v>3.1773535251626399E-2</v>
+      </c>
+      <c r="C159">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D159">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>2348.2249999999999</v>
+      </c>
+      <c r="B160">
+        <v>3.5044340351058599E-2</v>
+      </c>
+      <c r="C160">
+        <v>127.77225700164701</v>
+      </c>
+      <c r="D160">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>2363.56</v>
+      </c>
+      <c r="B161">
+        <v>3.2708050994321301E-2</v>
+      </c>
+      <c r="C161">
+        <v>127.721647446457</v>
+      </c>
+      <c r="D161">
+        <v>64.4488525390625</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>2378.8829999999998</v>
+      </c>
+      <c r="B162">
+        <v>3.08390195089315E-2</v>
+      </c>
+      <c r="C162">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D162">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>2394.2370000000001</v>
+      </c>
+      <c r="B163">
+        <v>2.9904503766236601E-2</v>
+      </c>
+      <c r="C163">
+        <v>127.780691927512</v>
+      </c>
+      <c r="D163">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>2409.5630000000001</v>
+      </c>
+      <c r="B164">
+        <v>3.2240793122973899E-2</v>
+      </c>
+      <c r="C164">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D164">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>2424.8980000000001</v>
+      </c>
+      <c r="B165">
+        <v>3.1306277380279003E-2</v>
+      </c>
+      <c r="C165">
+        <v>127.80599670510701</v>
+      </c>
+      <c r="D165">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>2440.2689999999998</v>
+      </c>
+      <c r="B166">
+        <v>3.4577082479711099E-2</v>
+      </c>
+      <c r="C166">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D166">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>2455.596</v>
+      </c>
+      <c r="B167">
+        <v>3.6913371836448397E-2</v>
+      </c>
+      <c r="C167">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D167">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>2470.9140000000002</v>
+      </c>
+      <c r="B168">
+        <v>3.5978856093753502E-2</v>
+      </c>
+      <c r="C168">
+        <v>127.730082372322</v>
+      </c>
+      <c r="D168">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>2486.2890000000002</v>
+      </c>
+      <c r="B169">
+        <v>3.2240793122973899E-2</v>
+      </c>
+      <c r="C169">
+        <v>127.73851729818701</v>
+      </c>
+      <c r="D169">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>2501.616</v>
+      </c>
+      <c r="B170">
+        <v>3.3175308865668801E-2</v>
+      </c>
+      <c r="C170">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D170">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>2516.953</v>
+      </c>
+      <c r="B171">
+        <v>3.3175308865668801E-2</v>
+      </c>
+      <c r="C171">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D171">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>2532.29</v>
+      </c>
+      <c r="B172">
+        <v>3.5978856093753502E-2</v>
+      </c>
+      <c r="C172">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D172">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>2547.6190000000001</v>
+      </c>
+      <c r="B173">
+        <v>3.5978856093753502E-2</v>
+      </c>
+      <c r="C173">
+        <v>127.77225700164701</v>
+      </c>
+      <c r="D173">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>2562.942</v>
+      </c>
+      <c r="B174">
+        <v>3.5978856093753502E-2</v>
+      </c>
+      <c r="C174">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D174">
+        <v>64.43115234375</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>2578.2910000000002</v>
+      </c>
+      <c r="B175">
+        <v>3.6446113965100897E-2</v>
+      </c>
+      <c r="C175">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D175">
+        <v>64.4134521484375</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>3289.1120000000001</v>
+      </c>
+      <c r="B176">
+        <v>4.4856755649354998E-2</v>
+      </c>
+      <c r="C176">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D176">
+        <v>64.395751953125</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>3304.4659999999999</v>
+      </c>
+      <c r="B177">
+        <v>5.0931107976871802E-2</v>
+      </c>
+      <c r="C177">
+        <v>127.77225700164701</v>
+      </c>
+      <c r="D177">
+        <v>64.395751953125</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>3319.7849999999999</v>
+      </c>
+      <c r="B178">
+        <v>5.1398365848219198E-2</v>
+      </c>
+      <c r="C178">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D178">
+        <v>64.395751953125</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>3335.1089999999999</v>
+      </c>
+      <c r="B179">
+        <v>4.6258529263397297E-2</v>
+      </c>
+      <c r="C179">
+        <v>127.746952224052</v>
+      </c>
+      <c r="D179">
+        <v>64.395751953125</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>3350.4670000000001</v>
+      </c>
+      <c r="B180">
+        <v>4.5791271392049901E-2</v>
+      </c>
+      <c r="C180">
+        <v>127.755387149917</v>
+      </c>
+      <c r="D180">
+        <v>64.3780517578125</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>3365.8090000000002</v>
+      </c>
+      <c r="B181">
+        <v>5.1865623719566697E-2</v>
+      </c>
+      <c r="C181">
+        <v>127.797561779242</v>
+      </c>
+      <c r="D181">
+        <v>64.3780517578125</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>3381.1289999999999</v>
+      </c>
+      <c r="B182">
+        <v>4.7660302877439699E-2</v>
+      </c>
+      <c r="C182">
+        <v>127.763822075782</v>
+      </c>
+      <c r="D182">
+        <v>64.395751953125</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>3396.4720000000002</v>
+      </c>
+      <c r="B183">
+        <v>4.6725787134744803E-2</v>
+      </c>
+      <c r="C183">
+        <v>127.789126853377</v>
+      </c>
+      <c r="D183">
+        <v>64.3780517578125</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>3411.797</v>
+      </c>
+      <c r="B184">
+        <v>5.1398365848219198E-2</v>
+      </c>
+      <c r="C184">
+        <v>127.789126853377</v>
+      </c>
+      <c r="D184">
+        <v>64.3780517578125</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>3427.1439999999998</v>
+      </c>
+      <c r="B185">
+        <v>5.28001394622616E-2</v>
+      </c>
+      <c r="C185">
+        <v>127.780691927512</v>
+      </c>
+      <c r="D185">
+        <v>64.3780517578125</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>3442.471</v>
+      </c>
+      <c r="B186">
+        <v>4.99965922341769E-2</v>
+      </c>
+      <c r="C186">
+        <v>127.789126853377</v>
+      </c>
+      <c r="D186">
+        <v>64.3780517578125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>